<commit_message>
Added "save to" button and text field that shows the path. Added output classes views (1st, 2nd...)
</commit_message>
<xml_diff>
--- a/src/Data/INPUT sample.xlsx
+++ b/src/Data/INPUT sample.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE73E15-F7EE-4B29-9AA8-AB02FEC35E1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6620C6-E9A6-4086-9F82-A1E9F2A550CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Professors" sheetId="1" r:id="rId1"/>
@@ -1270,7 +1270,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1621,7 +1621,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
@@ -2209,7 +2209,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3701,10 +3703,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4272,7 +4274,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f t="shared" ref="A12:A38" si="1">A11+1</f>
+        <f t="shared" ref="A12:A37" si="1">A11+1</f>
         <v>11</v>
       </c>
       <c r="B12">
@@ -5594,57 +5596,6 @@
       </c>
       <c r="P37">
         <v>-1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-      <c r="J38">
-        <v>-1</v>
-      </c>
-      <c r="K38">
-        <v>-1</v>
-      </c>
-      <c r="L38">
-        <v>1</v>
-      </c>
-      <c r="M38">
-        <v>1</v>
-      </c>
-      <c r="N38">
-        <v>0</v>
-      </c>
-      <c r="O38">
-        <v>1</v>
-      </c>
-      <c r="P38">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>